<commit_message>
So roda se tiver ~ na frente e adicionado msg de pronto e se ja estava pronto antes
</commit_message>
<xml_diff>
--- a/INFORMATIVO 5° GRE.xlsx
+++ b/INFORMATIVO 5° GRE.xlsx
@@ -471,11 +471,7 @@
           <t>NGI-7893</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -505,7 +501,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>~, 22, 22, 22, 22</t>
+          <t xml:space="preserve"> 22, 22, 22, 22</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -537,7 +533,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>~, 22, 22, 22, 22</t>
+          <t xml:space="preserve"> 22, 22, 22, 22</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -567,11 +563,7 @@
           <t>NHZ-5828</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -599,11 +591,7 @@
           <t>NHZ-5828</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -631,11 +619,7 @@
           <t>NHZ-5828</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -663,11 +647,7 @@
           <t>NIB-5967</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -695,11 +675,7 @@
           <t>NIB-5967</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -727,11 +703,7 @@
           <t>NIB-5967</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -759,11 +731,7 @@
           <t>NIB-5967</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -791,11 +759,7 @@
           <t>NIB-5967</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -823,11 +787,7 @@
           <t>NIB-5967</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -855,11 +815,7 @@
           <t>HZA-1907</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -889,7 +845,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>~, 22</t>
+          <t xml:space="preserve"> 22</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -919,11 +875,7 @@
           <t>HZA-1907</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -951,11 +903,7 @@
           <t>HZA-1907</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -983,11 +931,7 @@
           <t>HXY-3834</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1015,11 +959,7 @@
           <t>HXY-3834</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1047,11 +987,7 @@
           <t>HXY-3834</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1079,11 +1015,7 @@
           <t>HXY-3834</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1111,11 +1043,7 @@
           <t>NWS-3E07</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1143,11 +1071,7 @@
           <t>NWS-3E07</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1175,11 +1099,7 @@
           <t>NWS-3E07</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1207,11 +1127,7 @@
           <t>NWS-3E07</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1241,7 +1157,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>~, 22, 23, 22</t>
+          <t xml:space="preserve"> 22, 23, 22</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1271,11 +1187,7 @@
           <t>NGC-8763</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1303,11 +1215,7 @@
           <t>NGC-8763</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1335,11 +1243,7 @@
           <t>NGC-8763</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1367,11 +1271,7 @@
           <t>NWS-3453</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1399,11 +1299,7 @@
           <t>NWS-3453</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1431,11 +1327,7 @@
           <t>NWS-3453</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1463,11 +1355,7 @@
           <t>NWS-3453</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1495,11 +1383,7 @@
           <t>NGF-6733</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1527,11 +1411,7 @@
           <t>NGF-6733</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1559,11 +1439,7 @@
           <t>NNH-4900</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1591,11 +1467,7 @@
           <t>NNH-4900</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1623,11 +1495,7 @@
           <t>NNH-4900</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1655,11 +1523,7 @@
           <t>NNH-4900</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1687,11 +1551,7 @@
           <t>NIB-5997</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1719,11 +1579,7 @@
           <t>NIB-5997</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1751,11 +1607,7 @@
           <t>NIB-5997</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1783,11 +1635,7 @@
           <t>NIB-5997</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1815,11 +1663,7 @@
           <t>HZA-2317</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1847,11 +1691,7 @@
           <t>HZA-2317</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1879,11 +1719,7 @@
           <t>DTC-6607</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1911,11 +1747,7 @@
           <t>DTC-6607</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1943,11 +1775,7 @@
           <t>DTC-6607</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -1975,11 +1803,7 @@
           <t>DTC-6607</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2007,11 +1831,7 @@
           <t>NUP-8066</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2039,11 +1859,7 @@
           <t>NUP-8066</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2071,11 +1887,7 @@
           <t>NUP-8066</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2103,11 +1915,7 @@
           <t>NUP-8066</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2135,11 +1943,7 @@
           <t>HZA-1997</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2167,11 +1971,7 @@
           <t>HZA-1997</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2199,11 +1999,7 @@
           <t>HZA-1997</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2231,11 +2027,7 @@
           <t>HZA-1997</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2265,7 +2057,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>~, 22</t>
+          <t xml:space="preserve"> 22</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2295,11 +2087,7 @@
           <t>DJB-2167</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2327,11 +2115,7 @@
           <t>DJB-2167</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2359,11 +2143,7 @@
           <t>DJB-2167</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2391,11 +2171,7 @@
           <t>DJB-2167</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2423,11 +2199,7 @@
           <t>DJB-2167</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2455,11 +2227,7 @@
           <t>JRJ-6244</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2487,11 +2255,7 @@
           <t>JRJ-6244</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2519,11 +2283,7 @@
           <t>JRJ-6244</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2551,11 +2311,7 @@
           <t>JRJ-6244</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2583,11 +2339,7 @@
           <t>LWI-6376</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2615,11 +2367,7 @@
           <t>LWI-6376</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2647,11 +2395,7 @@
           <t>DJE-6560</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2679,11 +2423,7 @@
           <t>DJE-6560</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2711,11 +2451,7 @@
           <t>BXC-0096</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2743,11 +2479,7 @@
           <t>BXC-0096</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2775,11 +2507,7 @@
           <t>HYG-6364</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2807,11 +2535,7 @@
           <t>HYG-6364</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2839,11 +2563,7 @@
           <t>HYG-6364</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2871,11 +2591,7 @@
           <t>HYG-6364</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2903,11 +2619,7 @@
           <t>JRJ-6546</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2935,11 +2647,7 @@
           <t>JRJ-6546</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2967,11 +2675,7 @@
           <t>KHO7C77</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -2999,11 +2703,7 @@
           <t>KHO7C77</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -3031,11 +2731,7 @@
           <t>BXC-0096</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -3063,11 +2759,7 @@
           <t>BXC-0096</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -3097,7 +2789,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>~, 22</t>
+          <t xml:space="preserve"> 22</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3127,11 +2819,7 @@
           <t>NGC-8623</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B85" t="inlineStr"/>
       <c r="C85" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -3159,11 +2847,7 @@
           <t>NGC-8623</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -3191,11 +2875,7 @@
           <t>NGC-8623</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -3225,7 +2905,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>~, 22</t>
+          <t xml:space="preserve"> 22</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3255,11 +2935,7 @@
           <t>NGC-9103</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -3287,11 +2963,7 @@
           <t>NGC-9103</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr">
         <is>
           <t>MAIO</t>
@@ -3319,11 +2991,7 @@
           <t>NGC-9103</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
+      <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr">
         <is>
           <t>MAIO</t>

</xml_diff>